<commit_message>
Fixed CMS.12, CMS.27, and bug #221
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV_Production_Cards.xlsx
+++ b/conformancelib/testdata/PIV_Production_Cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GSA\GSA_GIT\piv-conformance-swing\conformancelib\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156DBB3F-6CD0-4048-9DD6-55D82C2D1F48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE2682A-E06B-479E-85A3-376E3704137A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="1620" windowWidth="28410" windowHeight="14550" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3680" uniqueCount="1273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3681" uniqueCount="1275">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3851,6 +3851,12 @@
   </si>
   <si>
     <t>PKIX_Test_28</t>
+  </si>
+  <si>
+    <t>2.16.840.1.101.3.6.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.3.6.1.1.16.4</t>
   </si>
 </sst>
 </file>
@@ -8472,8 +8478,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B417" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D440" sqref="D440"/>
+    <sheetView tabSelected="1" topLeftCell="B421" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C439" sqref="C439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -16526,8 +16532,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AMK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -20096,8 +20102,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:IV30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -21306,7 +21312,7 @@
   <dimension ref="A1:IV29"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:G29"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -21821,8 +21827,8 @@
       <c r="D13" s="30" t="s">
         <v>1028</v>
       </c>
-      <c r="E13" s="30" t="s">
-        <v>986</v>
+      <c r="E13" s="31" t="s">
+        <v>1273</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>759</v>
@@ -22116,7 +22122,9 @@
       <c r="D28" s="74" t="s">
         <v>586</v>
       </c>
-      <c r="E28" s="62"/>
+      <c r="E28" s="62" t="s">
+        <v>1274</v>
+      </c>
       <c r="F28" s="62"/>
       <c r="G28" s="62"/>
     </row>

</xml_diff>

<commit_message>
Cleaned up security object tests
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV_Production_Cards.xlsx
+++ b/conformancelib/testdata/PIV_Production_Cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\bf7450\git\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FB8C8D-1752-4C88-A117-13BE3657679F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C078D109-8AD3-4311-9BCF-D91BB807E477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="204" yWindow="0" windowWidth="23040" windowHeight="12360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6084" yWindow="0" windowWidth="23040" windowHeight="12360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps Overview" sheetId="2" r:id="rId1"/>
@@ -23,14 +23,14 @@
     <sheet name="Placeholders" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Steps Overview'!$C$1:$C$476</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Steps Overview'!$C$1:$C$474</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3078" uniqueCount="1291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3070" uniqueCount="1290">
   <si>
     <t>Card Capabilities Container</t>
   </si>
@@ -3791,12 +3791,6 @@
     <t>10.4.2.8</t>
   </si>
   <si>
-    <t>10.4.2.8.1</t>
-  </si>
-  <si>
-    <t>10.4.2.8.2</t>
-  </si>
-  <si>
     <t>10.5.1.6.1</t>
   </si>
   <si>
@@ -3903,6 +3897,9 @@
   </si>
   <si>
     <t>Message digest from signed attributes bag matches the digest over Facial Image biometric data (excluding contents of digital signature field)</t>
+  </si>
+  <si>
+    <t>The signature in the SignerInfo corresponds to the signed security object and that it is it signed with the certificate that is used to sign the CHUID.</t>
   </si>
 </sst>
 </file>
@@ -3976,7 +3973,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4039,6 +4036,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4143,7 +4146,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4346,6 +4349,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4735,10 +4741,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F489"/>
+  <dimension ref="A1:F487"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A292" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C301" sqref="C301"/>
+    <sheetView tabSelected="1" topLeftCell="A322" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A331" sqref="A331:XFD332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -4967,7 +4973,7 @@
         <v>78</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>79</v>
@@ -7482,7 +7488,7 @@
         <v>55</v>
       </c>
       <c r="B159" s="66" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="C159" s="41" t="s">
         <v>19</v>
@@ -7828,7 +7834,7 @@
         <v>55</v>
       </c>
       <c r="B179" s="66" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="C179" s="55" t="s">
         <v>22</v>
@@ -8156,7 +8162,7 @@
         <v>55</v>
       </c>
       <c r="B198" s="66" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="C198" s="41" t="s">
         <v>25</v>
@@ -8486,7 +8492,7 @@
         <v>55</v>
       </c>
       <c r="B217" s="66" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="C217" s="55" t="s">
         <v>311</v>
@@ -8992,7 +8998,7 @@
         <v>55</v>
       </c>
       <c r="B246" s="66" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="C246" s="41" t="s">
         <v>365</v>
@@ -10121,7 +10127,7 @@
         <v>450</v>
       </c>
       <c r="C312" s="25" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="D312" s="25" t="s">
         <v>901</v>
@@ -10425,114 +10431,118 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A330" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B330" s="66" t="s">
+    <row r="330" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+      <c r="A330" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="B330" s="68" t="s">
         <v>1252</v>
       </c>
-      <c r="C330" s="51" t="s">
-        <v>1242</v>
-      </c>
-      <c r="D330" s="51"/>
-      <c r="E330" s="59"/>
-      <c r="F330" s="59"/>
+      <c r="C330" s="68" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D330" s="68" t="s">
+        <v>406</v>
+      </c>
+      <c r="E330" s="68"/>
+      <c r="F330" s="25" t="s">
+        <v>1028</v>
+      </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A331" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B331" s="66" t="s">
-        <v>1253</v>
-      </c>
-      <c r="C331" s="25" t="s">
-        <v>1245</v>
-      </c>
-      <c r="D331" s="25" t="s">
-        <v>424</v>
-      </c>
-      <c r="E331" s="32"/>
-      <c r="F331" s="25" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="332" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+        <v>1202</v>
+      </c>
+      <c r="C331" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="D331" s="59"/>
+      <c r="E331" s="59"/>
+      <c r="F331" s="59"/>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A332" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B332" s="66" t="s">
-        <v>1254</v>
-      </c>
-      <c r="C332" s="25" t="s">
-        <v>426</v>
-      </c>
-      <c r="D332" s="25" t="s">
-        <v>1034</v>
-      </c>
-      <c r="E332" s="32"/>
-      <c r="F332" s="25" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A333" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="C332" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="D332" s="59"/>
+      <c r="E332" s="59"/>
+      <c r="F332" s="59"/>
+    </row>
+    <row r="333" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+      <c r="A333" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B333" s="66" t="s">
-        <v>1202</v>
-      </c>
-      <c r="C333" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="D333" s="59"/>
-      <c r="E333" s="59"/>
-      <c r="F333" s="59"/>
+        <v>479</v>
+      </c>
+      <c r="C333" s="25" t="s">
+        <v>410</v>
+      </c>
+      <c r="D333" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="E333" s="25"/>
+      <c r="F333" s="25" t="s">
+        <v>1154</v>
+      </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A334" s="25" t="s">
+      <c r="A334" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B334" s="66" t="s">
-        <v>478</v>
-      </c>
-      <c r="C334" s="61" t="s">
-        <v>35</v>
-      </c>
-      <c r="D334" s="59"/>
-      <c r="E334" s="59"/>
-      <c r="F334" s="59"/>
-    </row>
-    <row r="335" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+        <v>480</v>
+      </c>
+      <c r="C334" s="25" t="s">
+        <v>412</v>
+      </c>
+      <c r="D334" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="E334" s="25"/>
+      <c r="F334" s="25" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A335" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B335" s="66" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C335" s="25" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="D335" s="25" t="s">
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="E335" s="25"/>
       <c r="F335" s="25" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A336" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B336" s="66" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C336" s="25" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="D336" s="25" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="E336" s="25"/>
       <c r="F336" s="25" t="s">
@@ -10544,31 +10554,31 @@
         <v>55</v>
       </c>
       <c r="B337" s="66" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C337" s="25" t="s">
-        <v>414</v>
+        <v>386</v>
       </c>
       <c r="D337" s="25" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="E337" s="25"/>
       <c r="F337" s="25" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="338" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A338" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B338" s="66" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C338" s="25" t="s">
-        <v>416</v>
+        <v>389</v>
       </c>
       <c r="D338" s="25" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="E338" s="25"/>
       <c r="F338" s="25" t="s">
@@ -10580,13 +10590,13 @@
         <v>55</v>
       </c>
       <c r="B339" s="66" t="s">
-        <v>483</v>
+        <v>1253</v>
       </c>
       <c r="C339" s="25" t="s">
-        <v>386</v>
+        <v>420</v>
       </c>
       <c r="D339" s="25" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="E339" s="25"/>
       <c r="F339" s="25" t="s">
@@ -10598,13 +10608,13 @@
         <v>55</v>
       </c>
       <c r="B340" s="66" t="s">
-        <v>484</v>
+        <v>1254</v>
       </c>
       <c r="C340" s="25" t="s">
-        <v>389</v>
+        <v>422</v>
       </c>
       <c r="D340" s="25" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="E340" s="25"/>
       <c r="F340" s="25" t="s">
@@ -10616,63 +10626,63 @@
         <v>55</v>
       </c>
       <c r="B341" s="66" t="s">
-        <v>1255</v>
-      </c>
-      <c r="C341" s="25" t="s">
-        <v>420</v>
-      </c>
-      <c r="D341" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="E341" s="25"/>
-      <c r="F341" s="25" t="s">
-        <v>1154</v>
-      </c>
+        <v>1139</v>
+      </c>
+      <c r="C341" s="51" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D341" s="51"/>
+      <c r="E341" s="51"/>
+      <c r="F341" s="51"/>
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A342" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B342" s="66" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="C342" s="25" t="s">
-        <v>422</v>
+        <v>1251</v>
       </c>
       <c r="D342" s="25" t="s">
-        <v>398</v>
+        <v>424</v>
       </c>
       <c r="E342" s="25"/>
       <c r="F342" s="25" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A343" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B343" s="66" t="s">
-        <v>1139</v>
-      </c>
-      <c r="C343" s="51" t="s">
-        <v>1242</v>
-      </c>
-      <c r="D343" s="51"/>
-      <c r="E343" s="51"/>
-      <c r="F343" s="51"/>
-    </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1256</v>
+      </c>
+      <c r="C343" s="25" t="s">
+        <v>426</v>
+      </c>
+      <c r="D343" s="25" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E343" s="25"/>
+      <c r="F343" s="25" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A344" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B344" s="66" t="s">
-        <v>1257</v>
+        <v>1138</v>
       </c>
       <c r="C344" s="25" t="s">
-        <v>1251</v>
+        <v>428</v>
       </c>
       <c r="D344" s="25" t="s">
-        <v>424</v>
+        <v>901</v>
       </c>
       <c r="E344" s="25"/>
       <c r="F344" s="25" t="s">
@@ -10684,199 +10694,199 @@
         <v>55</v>
       </c>
       <c r="B345" s="66" t="s">
-        <v>1258</v>
+        <v>485</v>
       </c>
       <c r="C345" s="25" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="D345" s="25" t="s">
-        <v>1034</v>
+        <v>401</v>
       </c>
       <c r="E345" s="25"/>
       <c r="F345" s="25" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="346" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A346" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B346" s="66" t="s">
-        <v>1138</v>
-      </c>
-      <c r="C346" s="25" t="s">
-        <v>428</v>
+        <v>486</v>
+      </c>
+      <c r="C346" s="32" t="s">
+        <v>432</v>
       </c>
       <c r="D346" s="25" t="s">
-        <v>901</v>
+        <v>403</v>
       </c>
       <c r="E346" s="25"/>
       <c r="F346" s="25" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="347" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A347" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B347" s="66" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C347" s="25" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="D347" s="25" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="E347" s="25"/>
       <c r="F347" s="25" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="348" spans="1:6" ht="45" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A348" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B348" s="66" t="s">
-        <v>486</v>
-      </c>
-      <c r="C348" s="32" t="s">
-        <v>432</v>
+        <v>488</v>
+      </c>
+      <c r="C348" s="25" t="s">
+        <v>1248</v>
       </c>
       <c r="D348" s="25" t="s">
-        <v>403</v>
+        <v>436</v>
       </c>
       <c r="E348" s="25"/>
       <c r="F348" s="25" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="349" spans="1:6" ht="45" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A349" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B349" s="66" t="s">
-        <v>487</v>
-      </c>
-      <c r="C349" s="25" t="s">
-        <v>435</v>
+        <v>489</v>
+      </c>
+      <c r="C349" s="32" t="s">
+        <v>1159</v>
       </c>
       <c r="D349" s="25" t="s">
-        <v>406</v>
+        <v>1045</v>
       </c>
       <c r="E349" s="25"/>
       <c r="F349" s="25" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="350" spans="1:6" ht="30" x14ac:dyDescent="0.3">
-      <c r="A350" s="47" t="s">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A350" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B350" s="66" t="s">
-        <v>488</v>
-      </c>
-      <c r="C350" s="25" t="s">
-        <v>1248</v>
+        <v>490</v>
+      </c>
+      <c r="C350" s="32" t="s">
+        <v>1157</v>
       </c>
       <c r="D350" s="25" t="s">
-        <v>436</v>
+        <v>1048</v>
       </c>
       <c r="E350" s="25"/>
       <c r="F350" s="25" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A351" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="B351" s="66" t="s">
-        <v>489</v>
-      </c>
-      <c r="C351" s="32" t="s">
-        <v>1159</v>
-      </c>
-      <c r="D351" s="25" t="s">
-        <v>1045</v>
-      </c>
-      <c r="E351" s="25"/>
-      <c r="F351" s="25" t="s">
-        <v>1154</v>
-      </c>
+    <row r="351" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A351" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B351" s="65" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C351" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="D351" s="51"/>
+      <c r="E351" s="51"/>
+      <c r="F351" s="51"/>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A352" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B352" s="66" t="s">
-        <v>490</v>
-      </c>
-      <c r="C352" s="32" t="s">
-        <v>1157</v>
-      </c>
-      <c r="D352" s="25" t="s">
-        <v>1048</v>
-      </c>
-      <c r="E352" s="25"/>
-      <c r="F352" s="25" t="s">
-        <v>1154</v>
-      </c>
-    </row>
-    <row r="353" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A353" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="B353" s="65" t="s">
-        <v>1204</v>
+        <v>1203</v>
+      </c>
+      <c r="C352" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="D352" s="51"/>
+      <c r="E352" s="51"/>
+      <c r="F352" s="51"/>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A353" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B353" s="66" t="s">
+        <v>491</v>
       </c>
       <c r="C353" s="51" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D353" s="51"/>
       <c r="E353" s="51"/>
       <c r="F353" s="51"/>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:6" ht="60" x14ac:dyDescent="0.3">
       <c r="A354" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B354" s="66" t="s">
-        <v>1203</v>
-      </c>
-      <c r="C354" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="D354" s="51"/>
-      <c r="E354" s="51"/>
-      <c r="F354" s="51"/>
+        <v>492</v>
+      </c>
+      <c r="C354" s="32" t="s">
+        <v>493</v>
+      </c>
+      <c r="D354" s="25">
+        <v>78.3</v>
+      </c>
+      <c r="E354" s="25"/>
+      <c r="F354" s="25" t="s">
+        <v>1021</v>
+      </c>
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A355" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B355" s="66" t="s">
-        <v>491</v>
-      </c>
-      <c r="C355" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="D355" s="51"/>
-      <c r="E355" s="51"/>
-      <c r="F355" s="51"/>
-    </row>
-    <row r="356" spans="1:6" ht="60" x14ac:dyDescent="0.3">
+        <v>494</v>
+      </c>
+      <c r="C355" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="D355" s="25">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="E355" s="25"/>
+      <c r="F355" s="25" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A356" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B356" s="66" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="C356" s="32" t="s">
-        <v>493</v>
+        <v>1140</v>
       </c>
       <c r="D356" s="25">
-        <v>78.3</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="E356" s="25"/>
       <c r="F356" s="25" t="s">
@@ -10888,31 +10898,27 @@
         <v>55</v>
       </c>
       <c r="B357" s="66" t="s">
-        <v>494</v>
-      </c>
-      <c r="C357" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="D357" s="25">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E357" s="25"/>
-      <c r="F357" s="25" t="s">
-        <v>1021</v>
-      </c>
+        <v>498</v>
+      </c>
+      <c r="C357" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D357" s="51"/>
+      <c r="E357" s="51"/>
+      <c r="F357" s="51"/>
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A358" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B358" s="66" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="C358" s="32" t="s">
-        <v>1140</v>
-      </c>
-      <c r="D358" s="25">
-        <v>78.099999999999994</v>
+        <v>500</v>
+      </c>
+      <c r="D358" s="25" t="s">
+        <v>501</v>
       </c>
       <c r="E358" s="25"/>
       <c r="F358" s="25" t="s">
@@ -10924,27 +10930,31 @@
         <v>55</v>
       </c>
       <c r="B359" s="66" t="s">
-        <v>498</v>
-      </c>
-      <c r="C359" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="D359" s="51"/>
-      <c r="E359" s="51"/>
-      <c r="F359" s="51"/>
+        <v>502</v>
+      </c>
+      <c r="C359" s="32" t="s">
+        <v>503</v>
+      </c>
+      <c r="D359" s="25" t="s">
+        <v>504</v>
+      </c>
+      <c r="E359" s="25"/>
+      <c r="F359" s="25" t="s">
+        <v>1021</v>
+      </c>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A360" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B360" s="66" t="s">
-        <v>499</v>
-      </c>
-      <c r="C360" s="32" t="s">
-        <v>500</v>
+        <v>505</v>
+      </c>
+      <c r="C360" s="25" t="s">
+        <v>506</v>
       </c>
       <c r="D360" s="25" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="E360" s="25"/>
       <c r="F360" s="25" t="s">
@@ -10956,13 +10966,13 @@
         <v>55</v>
       </c>
       <c r="B361" s="66" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="C361" s="32" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="D361" s="25" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="E361" s="25"/>
       <c r="F361" s="25" t="s">
@@ -10974,31 +10984,27 @@
         <v>55</v>
       </c>
       <c r="B362" s="66" t="s">
-        <v>505</v>
-      </c>
-      <c r="C362" s="25" t="s">
-        <v>506</v>
-      </c>
-      <c r="D362" s="25" t="s">
-        <v>507</v>
-      </c>
-      <c r="E362" s="25"/>
-      <c r="F362" s="25" t="s">
-        <v>1021</v>
-      </c>
+        <v>511</v>
+      </c>
+      <c r="C362" s="51" t="s">
+        <v>512</v>
+      </c>
+      <c r="D362" s="51"/>
+      <c r="E362" s="51"/>
+      <c r="F362" s="51"/>
     </row>
     <row r="363" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A363" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B363" s="66" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="C363" s="32" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="D363" s="25" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="E363" s="25"/>
       <c r="F363" s="25" t="s">
@@ -11010,27 +11016,31 @@
         <v>55</v>
       </c>
       <c r="B364" s="66" t="s">
-        <v>511</v>
-      </c>
-      <c r="C364" s="51" t="s">
-        <v>512</v>
-      </c>
-      <c r="D364" s="51"/>
-      <c r="E364" s="51"/>
-      <c r="F364" s="51"/>
+        <v>516</v>
+      </c>
+      <c r="C364" s="32" t="s">
+        <v>517</v>
+      </c>
+      <c r="D364" s="25" t="s">
+        <v>518</v>
+      </c>
+      <c r="E364" s="25"/>
+      <c r="F364" s="25" t="s">
+        <v>1021</v>
+      </c>
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A365" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B365" s="66" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="C365" s="32" t="s">
-        <v>514</v>
+        <v>992</v>
       </c>
       <c r="D365" s="25" t="s">
-        <v>515</v>
+        <v>991</v>
       </c>
       <c r="E365" s="25"/>
       <c r="F365" s="25" t="s">
@@ -11042,33 +11052,33 @@
         <v>55</v>
       </c>
       <c r="B366" s="66" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="C366" s="32" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="D366" s="25" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="E366" s="25"/>
       <c r="F366" s="25" t="s">
         <v>1021</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A367" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B367" s="66" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
       <c r="C367" s="32" t="s">
-        <v>992</v>
+        <v>572</v>
       </c>
       <c r="D367" s="25" t="s">
-        <v>991</v>
-      </c>
-      <c r="E367" s="25"/>
+        <v>525</v>
+      </c>
+      <c r="E367" s="32"/>
       <c r="F367" s="25" t="s">
         <v>1021</v>
       </c>
@@ -11078,119 +11088,115 @@
         <v>55</v>
       </c>
       <c r="B368" s="66" t="s">
-        <v>521</v>
-      </c>
-      <c r="C368" s="32" t="s">
-        <v>522</v>
-      </c>
-      <c r="D368" s="25" t="s">
-        <v>523</v>
-      </c>
-      <c r="E368" s="25"/>
-      <c r="F368" s="25" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="369" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+        <v>526</v>
+      </c>
+      <c r="C368" s="51" t="s">
+        <v>527</v>
+      </c>
+      <c r="D368" s="51"/>
+      <c r="E368" s="51"/>
+      <c r="F368" s="51"/>
+    </row>
+    <row r="369" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A369" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B369" s="66" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="C369" s="32" t="s">
-        <v>572</v>
+        <v>530</v>
       </c>
       <c r="D369" s="25" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="E369" s="32"/>
       <c r="F369" s="25" t="s">
         <v>1021</v>
       </c>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A370" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B370" s="66" t="s">
-        <v>526</v>
-      </c>
-      <c r="C370" s="51" t="s">
-        <v>527</v>
-      </c>
-      <c r="D370" s="51"/>
-      <c r="E370" s="51"/>
-      <c r="F370" s="51"/>
-    </row>
-    <row r="371" spans="1:6" ht="45" x14ac:dyDescent="0.3">
+        <v>531</v>
+      </c>
+      <c r="C370" s="32" t="s">
+        <v>532</v>
+      </c>
+      <c r="D370" s="25" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E370" s="32"/>
+      <c r="F370" s="25" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A371" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B371" s="66" t="s">
-        <v>529</v>
+        <v>534</v>
       </c>
       <c r="C371" s="32" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
       <c r="D371" s="25" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
       <c r="E371" s="32"/>
       <c r="F371" s="25" t="s">
         <v>1021</v>
       </c>
     </row>
-    <row r="372" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A372" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B372" s="66" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="C372" s="32" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="D372" s="25" t="s">
-        <v>1162</v>
+        <v>539</v>
       </c>
       <c r="E372" s="32"/>
       <c r="F372" s="25" t="s">
         <v>1021</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A373" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B373" s="66" t="s">
-        <v>534</v>
-      </c>
-      <c r="C373" s="32" t="s">
-        <v>535</v>
-      </c>
-      <c r="D373" s="25" t="s">
-        <v>536</v>
-      </c>
-      <c r="E373" s="32"/>
-      <c r="F373" s="25" t="s">
-        <v>1021</v>
-      </c>
+        <v>540</v>
+      </c>
+      <c r="C373" s="51" t="s">
+        <v>541</v>
+      </c>
+      <c r="D373" s="51"/>
+      <c r="E373" s="51"/>
+      <c r="F373" s="51"/>
     </row>
     <row r="374" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A374" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B374" s="66" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="C374" s="32" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="D374" s="25" t="s">
-        <v>539</v>
-      </c>
-      <c r="E374" s="32"/>
+        <v>520</v>
+      </c>
+      <c r="E374" s="25"/>
       <c r="F374" s="25" t="s">
         <v>1021</v>
       </c>
@@ -11200,47 +11206,47 @@
         <v>55</v>
       </c>
       <c r="B375" s="66" t="s">
-        <v>540</v>
-      </c>
-      <c r="C375" s="51" t="s">
-        <v>541</v>
-      </c>
-      <c r="D375" s="51"/>
-      <c r="E375" s="51"/>
-      <c r="F375" s="51"/>
+        <v>544</v>
+      </c>
+      <c r="C375" s="25" t="s">
+        <v>545</v>
+      </c>
+      <c r="D375" s="25" t="s">
+        <v>988</v>
+      </c>
+      <c r="E375" s="25"/>
+      <c r="F375" s="25" t="s">
+        <v>1021</v>
+      </c>
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A376" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B376" s="66" t="s">
-        <v>542</v>
-      </c>
-      <c r="C376" s="32" t="s">
-        <v>543</v>
-      </c>
-      <c r="D376" s="25" t="s">
-        <v>520</v>
-      </c>
-      <c r="E376" s="25"/>
-      <c r="F376" s="25" t="s">
-        <v>1021</v>
-      </c>
+        <v>546</v>
+      </c>
+      <c r="C376" s="51" t="s">
+        <v>547</v>
+      </c>
+      <c r="D376" s="51"/>
+      <c r="E376" s="51"/>
+      <c r="F376" s="51"/>
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A377" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B377" s="66" t="s">
-        <v>544</v>
-      </c>
-      <c r="C377" s="25" t="s">
-        <v>545</v>
+        <v>548</v>
+      </c>
+      <c r="C377" s="32" t="s">
+        <v>514</v>
       </c>
       <c r="D377" s="25" t="s">
-        <v>988</v>
-      </c>
-      <c r="E377" s="25"/>
+        <v>515</v>
+      </c>
+      <c r="E377" s="32"/>
       <c r="F377" s="25" t="s">
         <v>1021</v>
       </c>
@@ -11250,27 +11256,31 @@
         <v>55</v>
       </c>
       <c r="B378" s="66" t="s">
-        <v>546</v>
-      </c>
-      <c r="C378" s="51" t="s">
-        <v>547</v>
-      </c>
-      <c r="D378" s="51"/>
-      <c r="E378" s="51"/>
-      <c r="F378" s="51"/>
+        <v>549</v>
+      </c>
+      <c r="C378" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="D378" s="25" t="s">
+        <v>993</v>
+      </c>
+      <c r="E378" s="32"/>
+      <c r="F378" s="25" t="s">
+        <v>1021</v>
+      </c>
     </row>
     <row r="379" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A379" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B379" s="66" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="C379" s="32" t="s">
-        <v>514</v>
+        <v>552</v>
       </c>
       <c r="D379" s="25" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="E379" s="32"/>
       <c r="F379" s="25" t="s">
@@ -11282,13 +11292,13 @@
         <v>55</v>
       </c>
       <c r="B380" s="66" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="C380" s="32" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D380" s="25" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="E380" s="32"/>
       <c r="F380" s="25" t="s">
@@ -11300,15 +11310,15 @@
         <v>55</v>
       </c>
       <c r="B381" s="66" t="s">
-        <v>551</v>
-      </c>
-      <c r="C381" s="32" t="s">
-        <v>552</v>
+        <v>555</v>
+      </c>
+      <c r="C381" s="25" t="s">
+        <v>556</v>
       </c>
       <c r="D381" s="25" t="s">
-        <v>520</v>
-      </c>
-      <c r="E381" s="32"/>
+        <v>989</v>
+      </c>
+      <c r="E381" s="25"/>
       <c r="F381" s="25" t="s">
         <v>1021</v>
       </c>
@@ -11318,77 +11328,77 @@
         <v>55</v>
       </c>
       <c r="B382" s="66" t="s">
-        <v>553</v>
-      </c>
-      <c r="C382" s="32" t="s">
-        <v>554</v>
-      </c>
-      <c r="D382" s="25" t="s">
-        <v>991</v>
-      </c>
-      <c r="E382" s="32"/>
-      <c r="F382" s="25" t="s">
-        <v>1021</v>
-      </c>
+        <v>1205</v>
+      </c>
+      <c r="C382" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D382" s="51"/>
+      <c r="E382" s="51"/>
+      <c r="F382" s="51"/>
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A383" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B383" s="66" t="s">
-        <v>555</v>
-      </c>
-      <c r="C383" s="25" t="s">
-        <v>556</v>
-      </c>
-      <c r="D383" s="25" t="s">
-        <v>989</v>
-      </c>
-      <c r="E383" s="25"/>
-      <c r="F383" s="25" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.3">
+        <v>557</v>
+      </c>
+      <c r="C383" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D383" s="51"/>
+      <c r="E383" s="51"/>
+      <c r="F383" s="51"/>
+    </row>
+    <row r="384" spans="1:6" ht="60" x14ac:dyDescent="0.3">
       <c r="A384" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B384" s="66" t="s">
-        <v>1205</v>
-      </c>
-      <c r="C384" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D384" s="51"/>
-      <c r="E384" s="51"/>
-      <c r="F384" s="51"/>
+        <v>558</v>
+      </c>
+      <c r="C384" s="32" t="s">
+        <v>493</v>
+      </c>
+      <c r="D384" s="25" t="s">
+        <v>929</v>
+      </c>
+      <c r="E384" s="32"/>
+      <c r="F384" s="25" t="s">
+        <v>1025</v>
+      </c>
     </row>
     <row r="385" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A385" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B385" s="66" t="s">
-        <v>557</v>
-      </c>
-      <c r="C385" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="D385" s="51"/>
-      <c r="E385" s="51"/>
-      <c r="F385" s="51"/>
-    </row>
-    <row r="386" spans="1:6" ht="60" x14ac:dyDescent="0.3">
+        <v>559</v>
+      </c>
+      <c r="C385" s="32" t="s">
+        <v>560</v>
+      </c>
+      <c r="D385" s="25" t="s">
+        <v>924</v>
+      </c>
+      <c r="E385" s="32"/>
+      <c r="F385" s="25" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A386" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B386" s="66" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="C386" s="32" t="s">
-        <v>493</v>
-      </c>
-      <c r="D386" s="25" t="s">
-        <v>929</v>
+        <v>497</v>
+      </c>
+      <c r="D386" s="25">
+        <v>78.099999999999994</v>
       </c>
       <c r="E386" s="32"/>
       <c r="F386" s="25" t="s">
@@ -11400,113 +11410,113 @@
         <v>55</v>
       </c>
       <c r="B387" s="66" t="s">
-        <v>559</v>
-      </c>
-      <c r="C387" s="32" t="s">
-        <v>560</v>
-      </c>
-      <c r="D387" s="25" t="s">
-        <v>924</v>
-      </c>
-      <c r="E387" s="32"/>
-      <c r="F387" s="25" t="s">
-        <v>1025</v>
-      </c>
+        <v>562</v>
+      </c>
+      <c r="C387" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D387" s="51"/>
+      <c r="E387" s="51"/>
+      <c r="F387" s="51"/>
     </row>
     <row r="388" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A388" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B388" s="66" t="s">
-        <v>561</v>
-      </c>
-      <c r="C388" s="32" t="s">
-        <v>497</v>
-      </c>
-      <c r="D388" s="25">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E388" s="32"/>
-      <c r="F388" s="25" t="s">
-        <v>1025</v>
-      </c>
+        <v>563</v>
+      </c>
+      <c r="C388" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="D388" s="51"/>
+      <c r="E388" s="51"/>
+      <c r="F388" s="51"/>
     </row>
     <row r="389" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A389" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B389" s="66" t="s">
-        <v>562</v>
-      </c>
-      <c r="C389" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="D389" s="51"/>
-      <c r="E389" s="51"/>
-      <c r="F389" s="51"/>
+        <v>565</v>
+      </c>
+      <c r="C389" s="25" t="s">
+        <v>566</v>
+      </c>
+      <c r="D389" s="25" t="s">
+        <v>567</v>
+      </c>
+      <c r="E389" s="32"/>
+      <c r="F389" s="25" t="s">
+        <v>1025</v>
+      </c>
     </row>
     <row r="390" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A390" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B390" s="66" t="s">
-        <v>563</v>
-      </c>
-      <c r="C390" s="51" t="s">
-        <v>564</v>
-      </c>
-      <c r="D390" s="51"/>
-      <c r="E390" s="51"/>
-      <c r="F390" s="51"/>
-    </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.3">
+        <v>568</v>
+      </c>
+      <c r="C390" s="32" t="s">
+        <v>569</v>
+      </c>
+      <c r="D390" s="25" t="s">
+        <v>570</v>
+      </c>
+      <c r="E390" s="32"/>
+      <c r="F390" s="25" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A391" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B391" s="66" t="s">
-        <v>565</v>
-      </c>
-      <c r="C391" s="25" t="s">
-        <v>566</v>
+        <v>571</v>
+      </c>
+      <c r="C391" s="32" t="s">
+        <v>572</v>
       </c>
       <c r="D391" s="25" t="s">
-        <v>567</v>
+        <v>525</v>
       </c>
       <c r="E391" s="32"/>
       <c r="F391" s="25" t="s">
         <v>1025</v>
       </c>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A392" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B392" s="66" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="C392" s="32" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="D392" s="25" t="s">
-        <v>570</v>
+        <v>536</v>
       </c>
       <c r="E392" s="32"/>
       <c r="F392" s="25" t="s">
         <v>1025</v>
       </c>
     </row>
-    <row r="393" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A393" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B393" s="66" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="C393" s="32" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="D393" s="25" t="s">
-        <v>525</v>
+        <v>539</v>
       </c>
       <c r="E393" s="32"/>
       <c r="F393" s="25" t="s">
@@ -11518,13 +11528,13 @@
         <v>55</v>
       </c>
       <c r="B394" s="66" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="C394" s="32" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="D394" s="25" t="s">
-        <v>536</v>
+        <v>510</v>
       </c>
       <c r="E394" s="32"/>
       <c r="F394" s="25" t="s">
@@ -11536,31 +11546,27 @@
         <v>55</v>
       </c>
       <c r="B395" s="66" t="s">
-        <v>575</v>
-      </c>
-      <c r="C395" s="32" t="s">
-        <v>576</v>
-      </c>
-      <c r="D395" s="25" t="s">
-        <v>539</v>
-      </c>
-      <c r="E395" s="32"/>
-      <c r="F395" s="25" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="396" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+        <v>579</v>
+      </c>
+      <c r="C395" s="51" t="s">
+        <v>541</v>
+      </c>
+      <c r="D395" s="51"/>
+      <c r="E395" s="51"/>
+      <c r="F395" s="51"/>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A396" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B396" s="66" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="C396" s="32" t="s">
-        <v>578</v>
+        <v>543</v>
       </c>
       <c r="D396" s="25" t="s">
-        <v>510</v>
+        <v>520</v>
       </c>
       <c r="E396" s="32"/>
       <c r="F396" s="25" t="s">
@@ -11572,47 +11578,47 @@
         <v>55</v>
       </c>
       <c r="B397" s="66" t="s">
-        <v>579</v>
-      </c>
-      <c r="C397" s="51" t="s">
-        <v>541</v>
-      </c>
-      <c r="D397" s="51"/>
-      <c r="E397" s="51"/>
-      <c r="F397" s="51"/>
+        <v>581</v>
+      </c>
+      <c r="C397" s="25" t="s">
+        <v>545</v>
+      </c>
+      <c r="D397" s="25" t="s">
+        <v>988</v>
+      </c>
+      <c r="E397" s="25"/>
+      <c r="F397" s="25" t="s">
+        <v>1025</v>
+      </c>
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A398" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B398" s="66" t="s">
-        <v>580</v>
-      </c>
-      <c r="C398" s="32" t="s">
-        <v>543</v>
-      </c>
-      <c r="D398" s="25" t="s">
-        <v>520</v>
-      </c>
-      <c r="E398" s="32"/>
-      <c r="F398" s="25" t="s">
-        <v>1025</v>
-      </c>
+        <v>582</v>
+      </c>
+      <c r="C398" s="51" t="s">
+        <v>547</v>
+      </c>
+      <c r="D398" s="51"/>
+      <c r="E398" s="51"/>
+      <c r="F398" s="51"/>
     </row>
     <row r="399" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A399" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B399" s="66" t="s">
-        <v>581</v>
-      </c>
-      <c r="C399" s="25" t="s">
-        <v>545</v>
+        <v>583</v>
+      </c>
+      <c r="C399" s="32" t="s">
+        <v>514</v>
       </c>
       <c r="D399" s="25" t="s">
-        <v>988</v>
-      </c>
-      <c r="E399" s="25"/>
+        <v>515</v>
+      </c>
+      <c r="E399" s="32"/>
       <c r="F399" s="25" t="s">
         <v>1025</v>
       </c>
@@ -11622,27 +11628,31 @@
         <v>55</v>
       </c>
       <c r="B400" s="66" t="s">
-        <v>582</v>
-      </c>
-      <c r="C400" s="51" t="s">
-        <v>547</v>
-      </c>
-      <c r="D400" s="51"/>
-      <c r="E400" s="51"/>
-      <c r="F400" s="51"/>
+        <v>584</v>
+      </c>
+      <c r="C400" s="32" t="s">
+        <v>585</v>
+      </c>
+      <c r="D400" s="25" t="s">
+        <v>993</v>
+      </c>
+      <c r="E400" s="32"/>
+      <c r="F400" s="25" t="s">
+        <v>1025</v>
+      </c>
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A401" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B401" s="66" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="C401" s="32" t="s">
-        <v>514</v>
+        <v>552</v>
       </c>
       <c r="D401" s="25" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="E401" s="32"/>
       <c r="F401" s="25" t="s">
@@ -11654,15 +11664,15 @@
         <v>55</v>
       </c>
       <c r="B402" s="66" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="C402" s="32" t="s">
-        <v>585</v>
+        <v>554</v>
       </c>
       <c r="D402" s="25" t="s">
-        <v>993</v>
-      </c>
-      <c r="E402" s="32"/>
+        <v>991</v>
+      </c>
+      <c r="E402" s="25"/>
       <c r="F402" s="25" t="s">
         <v>1025</v>
       </c>
@@ -11672,15 +11682,15 @@
         <v>55</v>
       </c>
       <c r="B403" s="66" t="s">
-        <v>586</v>
-      </c>
-      <c r="C403" s="32" t="s">
-        <v>552</v>
+        <v>588</v>
+      </c>
+      <c r="C403" s="25" t="s">
+        <v>556</v>
       </c>
       <c r="D403" s="25" t="s">
-        <v>520</v>
-      </c>
-      <c r="E403" s="32"/>
+        <v>989</v>
+      </c>
+      <c r="E403" s="25"/>
       <c r="F403" s="25" t="s">
         <v>1025</v>
       </c>
@@ -11690,77 +11700,77 @@
         <v>55</v>
       </c>
       <c r="B404" s="66" t="s">
-        <v>587</v>
-      </c>
-      <c r="C404" s="32" t="s">
-        <v>554</v>
-      </c>
-      <c r="D404" s="25" t="s">
-        <v>991</v>
-      </c>
-      <c r="E404" s="25"/>
-      <c r="F404" s="25" t="s">
-        <v>1025</v>
-      </c>
+        <v>1206</v>
+      </c>
+      <c r="C404" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="D404" s="51"/>
+      <c r="E404" s="51"/>
+      <c r="F404" s="51"/>
     </row>
     <row r="405" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A405" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B405" s="66" t="s">
-        <v>588</v>
-      </c>
-      <c r="C405" s="25" t="s">
-        <v>556</v>
-      </c>
-      <c r="D405" s="25" t="s">
-        <v>989</v>
-      </c>
-      <c r="E405" s="25"/>
-      <c r="F405" s="25" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.3">
+        <v>589</v>
+      </c>
+      <c r="C405" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D405" s="51"/>
+      <c r="E405" s="51"/>
+      <c r="F405" s="51"/>
+    </row>
+    <row r="406" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A406" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B406" s="66" t="s">
-        <v>1206</v>
-      </c>
-      <c r="C406" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D406" s="51"/>
-      <c r="E406" s="51"/>
-      <c r="F406" s="51"/>
+        <v>590</v>
+      </c>
+      <c r="C406" s="32" t="s">
+        <v>591</v>
+      </c>
+      <c r="D406" s="25">
+        <v>78.3</v>
+      </c>
+      <c r="E406" s="32"/>
+      <c r="F406" s="25" t="s">
+        <v>1026</v>
+      </c>
     </row>
     <row r="407" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A407" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B407" s="66" t="s">
-        <v>589</v>
-      </c>
-      <c r="C407" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="D407" s="51"/>
-      <c r="E407" s="51"/>
-      <c r="F407" s="51"/>
-    </row>
-    <row r="408" spans="1:6" ht="45" x14ac:dyDescent="0.3">
+        <v>592</v>
+      </c>
+      <c r="C407" s="25" t="s">
+        <v>593</v>
+      </c>
+      <c r="D407" s="25" t="s">
+        <v>924</v>
+      </c>
+      <c r="E407" s="25"/>
+      <c r="F407" s="25" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A408" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B408" s="66" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="C408" s="32" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="D408" s="25">
-        <v>78.3</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="E408" s="32"/>
       <c r="F408" s="25" t="s">
@@ -11772,95 +11782,95 @@
         <v>55</v>
       </c>
       <c r="B409" s="66" t="s">
-        <v>592</v>
-      </c>
-      <c r="C409" s="25" t="s">
-        <v>593</v>
-      </c>
-      <c r="D409" s="25" t="s">
-        <v>924</v>
-      </c>
-      <c r="E409" s="25"/>
-      <c r="F409" s="25" t="s">
-        <v>1026</v>
-      </c>
+        <v>596</v>
+      </c>
+      <c r="C409" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D409" s="51"/>
+      <c r="E409" s="51"/>
+      <c r="F409" s="51"/>
     </row>
     <row r="410" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A410" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B410" s="66" t="s">
-        <v>594</v>
-      </c>
-      <c r="C410" s="32" t="s">
-        <v>595</v>
-      </c>
-      <c r="D410" s="25">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E410" s="32"/>
-      <c r="F410" s="25" t="s">
-        <v>1026</v>
-      </c>
+        <v>597</v>
+      </c>
+      <c r="C410" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="D410" s="51"/>
+      <c r="E410" s="51"/>
+      <c r="F410" s="51"/>
     </row>
     <row r="411" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A411" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B411" s="66" t="s">
-        <v>596</v>
-      </c>
-      <c r="C411" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="D411" s="51"/>
-      <c r="E411" s="51"/>
-      <c r="F411" s="51"/>
+        <v>598</v>
+      </c>
+      <c r="C411" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="D411" s="25" t="s">
+        <v>963</v>
+      </c>
+      <c r="E411" s="32"/>
+      <c r="F411" s="25" t="s">
+        <v>1026</v>
+      </c>
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A412" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B412" s="66" t="s">
-        <v>597</v>
-      </c>
-      <c r="C412" s="51" t="s">
-        <v>564</v>
-      </c>
-      <c r="D412" s="51"/>
-      <c r="E412" s="51"/>
-      <c r="F412" s="51"/>
+        <v>600</v>
+      </c>
+      <c r="C412" s="32" t="s">
+        <v>601</v>
+      </c>
+      <c r="D412" s="25" t="s">
+        <v>602</v>
+      </c>
+      <c r="E412" s="32"/>
+      <c r="F412" s="25" t="s">
+        <v>1026</v>
+      </c>
     </row>
     <row r="413" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A413" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B413" s="66" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
       <c r="C413" s="32" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D413" s="25" t="s">
-        <v>963</v>
+        <v>504</v>
       </c>
       <c r="E413" s="32"/>
       <c r="F413" s="25" t="s">
         <v>1026</v>
       </c>
     </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A414" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B414" s="66" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="C414" s="32" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D414" s="25" t="s">
-        <v>602</v>
+        <v>525</v>
       </c>
       <c r="E414" s="32"/>
       <c r="F414" s="25" t="s">
@@ -11872,13 +11882,13 @@
         <v>55</v>
       </c>
       <c r="B415" s="66" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="C415" s="32" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="D415" s="25" t="s">
-        <v>504</v>
+        <v>539</v>
       </c>
       <c r="E415" s="32"/>
       <c r="F415" s="25" t="s">
@@ -11890,13 +11900,13 @@
         <v>55</v>
       </c>
       <c r="B416" s="66" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="C416" s="32" t="s">
-        <v>606</v>
+        <v>578</v>
       </c>
       <c r="D416" s="25" t="s">
-        <v>525</v>
+        <v>510</v>
       </c>
       <c r="E416" s="32"/>
       <c r="F416" s="25" t="s">
@@ -11908,31 +11918,27 @@
         <v>55</v>
       </c>
       <c r="B417" s="66" t="s">
-        <v>607</v>
-      </c>
-      <c r="C417" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="D417" s="25" t="s">
-        <v>539</v>
-      </c>
-      <c r="E417" s="32"/>
-      <c r="F417" s="25" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="418" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+        <v>610</v>
+      </c>
+      <c r="C417" s="51" t="s">
+        <v>541</v>
+      </c>
+      <c r="D417" s="51"/>
+      <c r="E417" s="51"/>
+      <c r="F417" s="51"/>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A418" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B418" s="66" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C418" s="32" t="s">
-        <v>578</v>
+        <v>543</v>
       </c>
       <c r="D418" s="25" t="s">
-        <v>510</v>
+        <v>520</v>
       </c>
       <c r="E418" s="32"/>
       <c r="F418" s="25" t="s">
@@ -11944,47 +11950,47 @@
         <v>55</v>
       </c>
       <c r="B419" s="66" t="s">
-        <v>610</v>
-      </c>
-      <c r="C419" s="51" t="s">
-        <v>541</v>
-      </c>
-      <c r="D419" s="51"/>
-      <c r="E419" s="51"/>
-      <c r="F419" s="51"/>
+        <v>612</v>
+      </c>
+      <c r="C419" s="25" t="s">
+        <v>545</v>
+      </c>
+      <c r="D419" s="25" t="s">
+        <v>988</v>
+      </c>
+      <c r="E419" s="25"/>
+      <c r="F419" s="25" t="s">
+        <v>1026</v>
+      </c>
     </row>
     <row r="420" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A420" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B420" s="66" t="s">
-        <v>611</v>
-      </c>
-      <c r="C420" s="32" t="s">
-        <v>543</v>
-      </c>
-      <c r="D420" s="25" t="s">
-        <v>520</v>
-      </c>
-      <c r="E420" s="32"/>
-      <c r="F420" s="25" t="s">
-        <v>1026</v>
-      </c>
+        <v>613</v>
+      </c>
+      <c r="C420" s="51" t="s">
+        <v>547</v>
+      </c>
+      <c r="D420" s="51"/>
+      <c r="E420" s="51"/>
+      <c r="F420" s="51"/>
     </row>
     <row r="421" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A421" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B421" s="66" t="s">
-        <v>612</v>
-      </c>
-      <c r="C421" s="25" t="s">
-        <v>545</v>
+        <v>614</v>
+      </c>
+      <c r="C421" s="32" t="s">
+        <v>514</v>
       </c>
       <c r="D421" s="25" t="s">
-        <v>988</v>
-      </c>
-      <c r="E421" s="25"/>
+        <v>515</v>
+      </c>
+      <c r="E421" s="32"/>
       <c r="F421" s="25" t="s">
         <v>1026</v>
       </c>
@@ -11994,27 +12000,31 @@
         <v>55</v>
       </c>
       <c r="B422" s="66" t="s">
-        <v>613</v>
-      </c>
-      <c r="C422" s="51" t="s">
-        <v>547</v>
-      </c>
-      <c r="D422" s="51"/>
-      <c r="E422" s="51"/>
-      <c r="F422" s="51"/>
+        <v>615</v>
+      </c>
+      <c r="C422" s="32" t="s">
+        <v>585</v>
+      </c>
+      <c r="D422" s="25" t="s">
+        <v>993</v>
+      </c>
+      <c r="E422" s="32"/>
+      <c r="F422" s="25" t="s">
+        <v>1026</v>
+      </c>
     </row>
     <row r="423" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A423" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B423" s="66" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="C423" s="32" t="s">
-        <v>514</v>
+        <v>552</v>
       </c>
       <c r="D423" s="25" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="E423" s="32"/>
       <c r="F423" s="25" t="s">
@@ -12026,15 +12036,15 @@
         <v>55</v>
       </c>
       <c r="B424" s="66" t="s">
-        <v>615</v>
-      </c>
-      <c r="C424" s="32" t="s">
-        <v>585</v>
+        <v>617</v>
+      </c>
+      <c r="C424" s="25" t="s">
+        <v>554</v>
       </c>
       <c r="D424" s="25" t="s">
-        <v>993</v>
-      </c>
-      <c r="E424" s="32"/>
+        <v>991</v>
+      </c>
+      <c r="E424" s="25"/>
       <c r="F424" s="25" t="s">
         <v>1026</v>
       </c>
@@ -12044,15 +12054,15 @@
         <v>55</v>
       </c>
       <c r="B425" s="66" t="s">
-        <v>616</v>
-      </c>
-      <c r="C425" s="32" t="s">
-        <v>552</v>
+        <v>618</v>
+      </c>
+      <c r="C425" s="25" t="s">
+        <v>556</v>
       </c>
       <c r="D425" s="25" t="s">
-        <v>520</v>
-      </c>
-      <c r="E425" s="32"/>
+        <v>989</v>
+      </c>
+      <c r="E425" s="25"/>
       <c r="F425" s="25" t="s">
         <v>1026</v>
       </c>
@@ -12062,77 +12072,77 @@
         <v>55</v>
       </c>
       <c r="B426" s="66" t="s">
-        <v>617</v>
-      </c>
-      <c r="C426" s="25" t="s">
-        <v>554</v>
-      </c>
-      <c r="D426" s="25" t="s">
-        <v>991</v>
-      </c>
-      <c r="E426" s="25"/>
-      <c r="F426" s="25" t="s">
-        <v>1026</v>
-      </c>
+        <v>1207</v>
+      </c>
+      <c r="C426" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D426" s="51"/>
+      <c r="E426" s="51"/>
+      <c r="F426" s="51"/>
     </row>
     <row r="427" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A427" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B427" s="66" t="s">
-        <v>618</v>
-      </c>
-      <c r="C427" s="25" t="s">
-        <v>556</v>
-      </c>
-      <c r="D427" s="25" t="s">
-        <v>989</v>
-      </c>
-      <c r="E427" s="25"/>
-      <c r="F427" s="25" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.3">
+        <v>619</v>
+      </c>
+      <c r="C427" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D427" s="51"/>
+      <c r="E427" s="51"/>
+      <c r="F427" s="51"/>
+    </row>
+    <row r="428" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A428" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B428" s="66" t="s">
-        <v>1207</v>
-      </c>
-      <c r="C428" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D428" s="51"/>
-      <c r="E428" s="51"/>
-      <c r="F428" s="51"/>
+        <v>620</v>
+      </c>
+      <c r="C428" s="32" t="s">
+        <v>591</v>
+      </c>
+      <c r="D428" s="25">
+        <v>78.3</v>
+      </c>
+      <c r="E428" s="32"/>
+      <c r="F428" s="25" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="429" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A429" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B429" s="66" t="s">
-        <v>619</v>
-      </c>
-      <c r="C429" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="D429" s="51"/>
-      <c r="E429" s="51"/>
-      <c r="F429" s="51"/>
-    </row>
-    <row r="430" spans="1:6" ht="45" x14ac:dyDescent="0.3">
+        <v>621</v>
+      </c>
+      <c r="C429" s="32" t="s">
+        <v>622</v>
+      </c>
+      <c r="D429" s="25">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="E429" s="32"/>
+      <c r="F429" s="25" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A430" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B430" s="66" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="C430" s="32" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="D430" s="25">
-        <v>78.3</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="E430" s="32"/>
       <c r="F430" s="25" t="s">
@@ -12144,79 +12154,79 @@
         <v>55</v>
       </c>
       <c r="B431" s="66" t="s">
-        <v>621</v>
-      </c>
-      <c r="C431" s="32" t="s">
-        <v>622</v>
-      </c>
-      <c r="D431" s="25">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E431" s="32"/>
-      <c r="F431" s="25" t="s">
-        <v>1027</v>
-      </c>
+        <v>624</v>
+      </c>
+      <c r="C431" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D431" s="51"/>
+      <c r="E431" s="51"/>
+      <c r="F431" s="51"/>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A432" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B432" s="66" t="s">
-        <v>623</v>
-      </c>
-      <c r="C432" s="32" t="s">
-        <v>595</v>
-      </c>
-      <c r="D432" s="25">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E432" s="32"/>
-      <c r="F432" s="25" t="s">
-        <v>1027</v>
-      </c>
+        <v>625</v>
+      </c>
+      <c r="C432" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="D432" s="51"/>
+      <c r="E432" s="51"/>
+      <c r="F432" s="51"/>
     </row>
     <row r="433" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A433" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B433" s="66" t="s">
-        <v>624</v>
-      </c>
-      <c r="C433" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="D433" s="51"/>
-      <c r="E433" s="51"/>
-      <c r="F433" s="51"/>
+        <v>626</v>
+      </c>
+      <c r="C433" s="25" t="s">
+        <v>566</v>
+      </c>
+      <c r="D433" s="25" t="s">
+        <v>567</v>
+      </c>
+      <c r="E433" s="25"/>
+      <c r="F433" s="25" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="434" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A434" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B434" s="66" t="s">
-        <v>625</v>
-      </c>
-      <c r="C434" s="51" t="s">
-        <v>564</v>
-      </c>
-      <c r="D434" s="51"/>
-      <c r="E434" s="51"/>
-      <c r="F434" s="51"/>
+        <v>627</v>
+      </c>
+      <c r="C434" s="32" t="s">
+        <v>628</v>
+      </c>
+      <c r="D434" s="25" t="s">
+        <v>501</v>
+      </c>
+      <c r="E434" s="32"/>
+      <c r="F434" s="25" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="435" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A435" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B435" s="66" t="s">
-        <v>626</v>
-      </c>
-      <c r="C435" s="25" t="s">
-        <v>566</v>
+        <v>629</v>
+      </c>
+      <c r="C435" s="32" t="s">
+        <v>630</v>
       </c>
       <c r="D435" s="25" t="s">
-        <v>567</v>
-      </c>
-      <c r="E435" s="25"/>
+        <v>504</v>
+      </c>
+      <c r="E435" s="32"/>
       <c r="F435" s="25" t="s">
         <v>1027</v>
       </c>
@@ -12226,15 +12236,15 @@
         <v>55</v>
       </c>
       <c r="B436" s="66" t="s">
-        <v>627</v>
-      </c>
-      <c r="C436" s="32" t="s">
-        <v>628</v>
+        <v>631</v>
+      </c>
+      <c r="C436" s="25" t="s">
+        <v>632</v>
       </c>
       <c r="D436" s="25" t="s">
-        <v>501</v>
-      </c>
-      <c r="E436" s="32"/>
+        <v>510</v>
+      </c>
+      <c r="E436" s="25"/>
       <c r="F436" s="25" t="s">
         <v>1027</v>
       </c>
@@ -12244,31 +12254,27 @@
         <v>55</v>
       </c>
       <c r="B437" s="66" t="s">
-        <v>629</v>
-      </c>
-      <c r="C437" s="32" t="s">
-        <v>630</v>
-      </c>
-      <c r="D437" s="25" t="s">
-        <v>504</v>
-      </c>
-      <c r="E437" s="32"/>
-      <c r="F437" s="25" t="s">
-        <v>1027</v>
-      </c>
+        <v>633</v>
+      </c>
+      <c r="C437" s="51" t="s">
+        <v>634</v>
+      </c>
+      <c r="D437" s="51"/>
+      <c r="E437" s="51"/>
+      <c r="F437" s="51"/>
     </row>
     <row r="438" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A438" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B438" s="66" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="C438" s="25" t="s">
-        <v>632</v>
+        <v>1147</v>
       </c>
       <c r="D438" s="25" t="s">
-        <v>510</v>
+        <v>636</v>
       </c>
       <c r="E438" s="25"/>
       <c r="F438" s="25" t="s">
@@ -12280,27 +12286,31 @@
         <v>55</v>
       </c>
       <c r="B439" s="66" t="s">
-        <v>633</v>
-      </c>
-      <c r="C439" s="51" t="s">
-        <v>634</v>
-      </c>
-      <c r="D439" s="51"/>
-      <c r="E439" s="51"/>
-      <c r="F439" s="51"/>
+        <v>637</v>
+      </c>
+      <c r="C439" s="25" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D439" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="E439" s="25"/>
+      <c r="F439" s="25" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="440" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A440" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B440" s="66" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="C440" s="25" t="s">
-        <v>1147</v>
+        <v>640</v>
       </c>
       <c r="D440" s="25" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="E440" s="25"/>
       <c r="F440" s="25" t="s">
@@ -12312,33 +12322,29 @@
         <v>55</v>
       </c>
       <c r="B441" s="66" t="s">
-        <v>637</v>
-      </c>
-      <c r="C441" s="25" t="s">
-        <v>1146</v>
-      </c>
-      <c r="D441" s="25" t="s">
-        <v>638</v>
-      </c>
-      <c r="E441" s="25"/>
-      <c r="F441" s="25" t="s">
-        <v>1027</v>
-      </c>
+        <v>641</v>
+      </c>
+      <c r="C441" s="51" t="s">
+        <v>547</v>
+      </c>
+      <c r="D441" s="51"/>
+      <c r="E441" s="51"/>
+      <c r="F441" s="51"/>
     </row>
     <row r="442" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A442" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B442" s="66" t="s">
-        <v>639</v>
-      </c>
-      <c r="C442" s="25" t="s">
-        <v>640</v>
+        <v>642</v>
+      </c>
+      <c r="C442" s="32" t="s">
+        <v>514</v>
       </c>
       <c r="D442" s="25" t="s">
-        <v>638</v>
-      </c>
-      <c r="E442" s="25"/>
+        <v>515</v>
+      </c>
+      <c r="E442" s="32"/>
       <c r="F442" s="25" t="s">
         <v>1027</v>
       </c>
@@ -12348,27 +12354,31 @@
         <v>55</v>
       </c>
       <c r="B443" s="66" t="s">
-        <v>641</v>
-      </c>
-      <c r="C443" s="51" t="s">
-        <v>547</v>
-      </c>
-      <c r="D443" s="51"/>
-      <c r="E443" s="51"/>
-      <c r="F443" s="51"/>
+        <v>643</v>
+      </c>
+      <c r="C443" s="32" t="s">
+        <v>644</v>
+      </c>
+      <c r="D443" s="25" t="s">
+        <v>518</v>
+      </c>
+      <c r="E443" s="32"/>
+      <c r="F443" s="25" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="444" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A444" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B444" s="66" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="C444" s="32" t="s">
-        <v>514</v>
+        <v>552</v>
       </c>
       <c r="D444" s="25" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="E444" s="32"/>
       <c r="F444" s="25" t="s">
@@ -12380,15 +12390,15 @@
         <v>55</v>
       </c>
       <c r="B445" s="66" t="s">
-        <v>643</v>
-      </c>
-      <c r="C445" s="32" t="s">
-        <v>644</v>
+        <v>646</v>
+      </c>
+      <c r="C445" s="25" t="s">
+        <v>554</v>
       </c>
       <c r="D445" s="25" t="s">
-        <v>518</v>
-      </c>
-      <c r="E445" s="32"/>
+        <v>520</v>
+      </c>
+      <c r="E445" s="25"/>
       <c r="F445" s="25" t="s">
         <v>1027</v>
       </c>
@@ -12398,33 +12408,33 @@
         <v>55</v>
       </c>
       <c r="B446" s="66" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="C446" s="32" t="s">
-        <v>552</v>
+        <v>522</v>
       </c>
       <c r="D446" s="25" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="E446" s="32"/>
       <c r="F446" s="25" t="s">
         <v>1027</v>
       </c>
     </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A447" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B447" s="66" t="s">
-        <v>646</v>
-      </c>
-      <c r="C447" s="25" t="s">
-        <v>554</v>
+        <v>648</v>
+      </c>
+      <c r="C447" s="32" t="s">
+        <v>606</v>
       </c>
       <c r="D447" s="25" t="s">
-        <v>520</v>
-      </c>
-      <c r="E447" s="25"/>
+        <v>525</v>
+      </c>
+      <c r="E447" s="32"/>
       <c r="F447" s="25" t="s">
         <v>1027</v>
       </c>
@@ -12434,81 +12444,81 @@
         <v>55</v>
       </c>
       <c r="B448" s="66" t="s">
-        <v>647</v>
-      </c>
-      <c r="C448" s="32" t="s">
-        <v>522</v>
-      </c>
-      <c r="D448" s="25" t="s">
-        <v>523</v>
-      </c>
-      <c r="E448" s="32"/>
-      <c r="F448" s="25" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="449" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+        <v>649</v>
+      </c>
+      <c r="C448" s="51" t="s">
+        <v>527</v>
+      </c>
+      <c r="D448" s="51"/>
+      <c r="E448" s="51"/>
+      <c r="F448" s="51"/>
+    </row>
+    <row r="449" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A449" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B449" s="66" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="C449" s="32" t="s">
-        <v>606</v>
+        <v>530</v>
       </c>
       <c r="D449" s="25" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="E449" s="32"/>
       <c r="F449" s="25" t="s">
         <v>1027</v>
       </c>
     </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A450" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B450" s="66" t="s">
-        <v>649</v>
-      </c>
-      <c r="C450" s="51" t="s">
-        <v>527</v>
-      </c>
-      <c r="D450" s="51"/>
-      <c r="E450" s="51"/>
-      <c r="F450" s="51"/>
-    </row>
-    <row r="451" spans="1:6" ht="45" x14ac:dyDescent="0.3">
+        <v>651</v>
+      </c>
+      <c r="C450" s="32" t="s">
+        <v>532</v>
+      </c>
+      <c r="D450" s="25" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E450" s="32"/>
+      <c r="F450" s="25" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A451" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B451" s="66" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="C451" s="32" t="s">
-        <v>530</v>
+        <v>653</v>
       </c>
       <c r="D451" s="25" t="s">
-        <v>528</v>
+        <v>1164</v>
       </c>
       <c r="E451" s="32"/>
       <c r="F451" s="25" t="s">
         <v>1027</v>
       </c>
     </row>
-    <row r="452" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A452" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B452" s="66" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="C452" s="32" t="s">
-        <v>532</v>
+        <v>608</v>
       </c>
       <c r="D452" s="25" t="s">
-        <v>1162</v>
+        <v>539</v>
       </c>
       <c r="E452" s="32"/>
       <c r="F452" s="25" t="s">
@@ -12520,31 +12530,27 @@
         <v>55</v>
       </c>
       <c r="B453" s="66" t="s">
-        <v>652</v>
-      </c>
-      <c r="C453" s="32" t="s">
-        <v>653</v>
-      </c>
-      <c r="D453" s="25" t="s">
-        <v>1164</v>
-      </c>
-      <c r="E453" s="32"/>
-      <c r="F453" s="25" t="s">
-        <v>1027</v>
-      </c>
+        <v>655</v>
+      </c>
+      <c r="C453" s="51" t="s">
+        <v>541</v>
+      </c>
+      <c r="D453" s="51"/>
+      <c r="E453" s="51"/>
+      <c r="F453" s="51"/>
     </row>
     <row r="454" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A454" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B454" s="66" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="C454" s="32" t="s">
-        <v>608</v>
+        <v>543</v>
       </c>
       <c r="D454" s="25" t="s">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="E454" s="32"/>
       <c r="F454" s="25" t="s">
@@ -12556,45 +12562,45 @@
         <v>55</v>
       </c>
       <c r="B455" s="66" t="s">
-        <v>655</v>
-      </c>
-      <c r="C455" s="51" t="s">
-        <v>541</v>
-      </c>
-      <c r="D455" s="51"/>
-      <c r="E455" s="51"/>
-      <c r="F455" s="51"/>
+        <v>657</v>
+      </c>
+      <c r="C455" s="25" t="s">
+        <v>545</v>
+      </c>
+      <c r="D455" s="25" t="s">
+        <v>988</v>
+      </c>
+      <c r="E455" s="25"/>
+      <c r="F455" s="25" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="456" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A456" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B456" s="66" t="s">
-        <v>656</v>
-      </c>
-      <c r="C456" s="32" t="s">
-        <v>543</v>
-      </c>
-      <c r="D456" s="25" t="s">
-        <v>520</v>
-      </c>
-      <c r="E456" s="32"/>
-      <c r="F456" s="25" t="s">
-        <v>1027</v>
-      </c>
+        <v>658</v>
+      </c>
+      <c r="C456" s="51" t="s">
+        <v>998</v>
+      </c>
+      <c r="D456" s="51"/>
+      <c r="E456" s="51"/>
+      <c r="F456" s="51"/>
     </row>
     <row r="457" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A457" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B457" s="66" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="C457" s="25" t="s">
-        <v>545</v>
+        <v>556</v>
       </c>
       <c r="D457" s="25" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E457" s="25"/>
       <c r="F457" s="25" t="s">
@@ -12606,13 +12612,13 @@
         <v>55</v>
       </c>
       <c r="B458" s="66" t="s">
-        <v>658</v>
-      </c>
-      <c r="C458" s="51" t="s">
-        <v>998</v>
+        <v>1208</v>
+      </c>
+      <c r="C458" s="41" t="s">
+        <v>46</v>
       </c>
       <c r="D458" s="51"/>
-      <c r="E458" s="51"/>
+      <c r="E458" s="41"/>
       <c r="F458" s="51"/>
     </row>
     <row r="459" spans="1:6" x14ac:dyDescent="0.3">
@@ -12620,17 +12626,15 @@
         <v>55</v>
       </c>
       <c r="B459" s="66" t="s">
-        <v>659</v>
-      </c>
-      <c r="C459" s="25" t="s">
-        <v>556</v>
-      </c>
-      <c r="D459" s="25" t="s">
-        <v>989</v>
-      </c>
-      <c r="E459" s="25"/>
+        <v>660</v>
+      </c>
+      <c r="C459" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D459" s="25"/>
+      <c r="E459" s="32"/>
       <c r="F459" s="25" t="s">
-        <v>1027</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="460" spans="1:6" x14ac:dyDescent="0.3">
@@ -12638,29 +12642,31 @@
         <v>55</v>
       </c>
       <c r="B460" s="66" t="s">
-        <v>1208</v>
-      </c>
-      <c r="C460" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D460" s="51"/>
-      <c r="E460" s="41"/>
-      <c r="F460" s="51"/>
+        <v>661</v>
+      </c>
+      <c r="C460" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D460" s="25"/>
+      <c r="E460" s="32"/>
+      <c r="F460" s="25" t="s">
+        <v>1279</v>
+      </c>
     </row>
     <row r="461" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A461" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B461" s="66" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="C461" s="32" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D461" s="25"/>
       <c r="E461" s="32"/>
       <c r="F461" s="25" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="462" spans="1:6" x14ac:dyDescent="0.3">
@@ -12668,115 +12674,119 @@
         <v>55</v>
       </c>
       <c r="B462" s="66" t="s">
-        <v>661</v>
-      </c>
-      <c r="C462" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="D462" s="25"/>
-      <c r="E462" s="32"/>
-      <c r="F462" s="25" t="s">
-        <v>1281</v>
-      </c>
+        <v>1209</v>
+      </c>
+      <c r="C462" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D462" s="51"/>
+      <c r="E462" s="41"/>
+      <c r="F462" s="51"/>
     </row>
     <row r="463" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A463" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B463" s="66" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C463" s="32" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D463" s="25"/>
       <c r="E463" s="32"/>
-      <c r="F463" s="25" t="s">
-        <v>1281</v>
-      </c>
+      <c r="F463" s="25"/>
     </row>
     <row r="464" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A464" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B464" s="66" t="s">
-        <v>1209</v>
-      </c>
-      <c r="C464" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="D464" s="51"/>
-      <c r="E464" s="41"/>
-      <c r="F464" s="51"/>
+        <v>664</v>
+      </c>
+      <c r="C464" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D464" s="25"/>
+      <c r="E464" s="32"/>
+      <c r="F464" s="25"/>
     </row>
     <row r="465" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A465" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B465" s="66" t="s">
-        <v>663</v>
-      </c>
-      <c r="C465" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="D465" s="25"/>
-      <c r="E465" s="32"/>
-      <c r="F465" s="25"/>
+        <v>1257</v>
+      </c>
+      <c r="C465" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D465" s="51"/>
+      <c r="E465" s="41"/>
+      <c r="F465" s="51"/>
     </row>
     <row r="466" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A466" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B466" s="66" t="s">
-        <v>664</v>
-      </c>
-      <c r="C466" s="32" t="s">
+        <v>665</v>
+      </c>
+      <c r="C466" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="D466" s="25"/>
-      <c r="E466" s="32"/>
-      <c r="F466" s="25"/>
-    </row>
-    <row r="467" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D466" s="51"/>
+      <c r="E466" s="51"/>
+      <c r="F466" s="51"/>
+    </row>
+    <row r="467" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A467" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B467" s="66" t="s">
-        <v>1259</v>
-      </c>
-      <c r="C467" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="D467" s="51"/>
-      <c r="E467" s="41"/>
-      <c r="F467" s="51"/>
+        <v>666</v>
+      </c>
+      <c r="C467" s="32" t="s">
+        <v>591</v>
+      </c>
+      <c r="D467" s="25">
+        <v>78.3</v>
+      </c>
+      <c r="E467" s="32"/>
+      <c r="F467" s="25" t="s">
+        <v>1020</v>
+      </c>
     </row>
     <row r="468" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A468" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B468" s="66" t="s">
-        <v>665</v>
-      </c>
-      <c r="C468" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="D468" s="51"/>
-      <c r="E468" s="51"/>
-      <c r="F468" s="51"/>
-    </row>
-    <row r="469" spans="1:6" ht="45" x14ac:dyDescent="0.3">
+        <v>667</v>
+      </c>
+      <c r="C468" s="32" t="s">
+        <v>622</v>
+      </c>
+      <c r="D468" s="25">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="E468" s="32"/>
+      <c r="F468" s="25" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="469" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A469" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B469" s="66" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="C469" s="32" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="D469" s="25">
-        <v>78.3</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="E469" s="32"/>
       <c r="F469" s="25" t="s">
@@ -12788,79 +12798,79 @@
         <v>55</v>
       </c>
       <c r="B470" s="66" t="s">
-        <v>667</v>
-      </c>
-      <c r="C470" s="32" t="s">
-        <v>622</v>
-      </c>
-      <c r="D470" s="25">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E470" s="32"/>
-      <c r="F470" s="25" t="s">
-        <v>1020</v>
-      </c>
+        <v>669</v>
+      </c>
+      <c r="C470" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D470" s="51"/>
+      <c r="E470" s="51"/>
+      <c r="F470" s="51"/>
     </row>
     <row r="471" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A471" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B471" s="66" t="s">
-        <v>668</v>
-      </c>
-      <c r="C471" s="32" t="s">
-        <v>595</v>
-      </c>
-      <c r="D471" s="25">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E471" s="32"/>
-      <c r="F471" s="25" t="s">
-        <v>1020</v>
-      </c>
+        <v>670</v>
+      </c>
+      <c r="C471" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="D471" s="51"/>
+      <c r="E471" s="51"/>
+      <c r="F471" s="51"/>
     </row>
     <row r="472" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A472" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B472" s="66" t="s">
-        <v>669</v>
-      </c>
-      <c r="C472" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="D472" s="51"/>
-      <c r="E472" s="51"/>
-      <c r="F472" s="51"/>
+        <v>671</v>
+      </c>
+      <c r="C472" s="32" t="s">
+        <v>672</v>
+      </c>
+      <c r="D472" s="25" t="s">
+        <v>501</v>
+      </c>
+      <c r="E472" s="32"/>
+      <c r="F472" s="25" t="s">
+        <v>1020</v>
+      </c>
     </row>
     <row r="473" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A473" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B473" s="66" t="s">
-        <v>670</v>
-      </c>
-      <c r="C473" s="51" t="s">
-        <v>564</v>
-      </c>
-      <c r="D473" s="51"/>
-      <c r="E473" s="51"/>
-      <c r="F473" s="51"/>
+        <v>673</v>
+      </c>
+      <c r="C473" s="32" t="s">
+        <v>630</v>
+      </c>
+      <c r="D473" s="25" t="s">
+        <v>504</v>
+      </c>
+      <c r="E473" s="32"/>
+      <c r="F473" s="25" t="s">
+        <v>1020</v>
+      </c>
     </row>
     <row r="474" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A474" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B474" s="66" t="s">
-        <v>671</v>
-      </c>
-      <c r="C474" s="32" t="s">
-        <v>672</v>
+        <v>674</v>
+      </c>
+      <c r="C474" s="25" t="s">
+        <v>675</v>
       </c>
       <c r="D474" s="25" t="s">
-        <v>501</v>
-      </c>
-      <c r="E474" s="32"/>
+        <v>990</v>
+      </c>
+      <c r="E474" s="25"/>
       <c r="F474" s="25" t="s">
         <v>1020</v>
       </c>
@@ -12870,15 +12880,15 @@
         <v>55</v>
       </c>
       <c r="B475" s="66" t="s">
-        <v>673</v>
-      </c>
-      <c r="C475" s="32" t="s">
-        <v>630</v>
+        <v>676</v>
+      </c>
+      <c r="C475" s="25" t="s">
+        <v>677</v>
       </c>
       <c r="D475" s="25" t="s">
-        <v>504</v>
-      </c>
-      <c r="E475" s="32"/>
+        <v>539</v>
+      </c>
+      <c r="E475" s="25"/>
       <c r="F475" s="25" t="s">
         <v>1020</v>
       </c>
@@ -12888,31 +12898,29 @@
         <v>55</v>
       </c>
       <c r="B476" s="66" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="C476" s="25" t="s">
-        <v>675</v>
-      </c>
-      <c r="D476" s="25" t="s">
-        <v>990</v>
-      </c>
+        <v>1006</v>
+      </c>
+      <c r="D476" s="25"/>
       <c r="E476" s="25"/>
       <c r="F476" s="25" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="477" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A477" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B477" s="66" t="s">
-        <v>676</v>
+        <v>1007</v>
       </c>
       <c r="C477" s="25" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="D477" s="25" t="s">
-        <v>539</v>
+        <v>510</v>
       </c>
       <c r="E477" s="25"/>
       <c r="F477" s="25" t="s">
@@ -12924,49 +12932,47 @@
         <v>55</v>
       </c>
       <c r="B478" s="66" t="s">
-        <v>678</v>
+        <v>1008</v>
       </c>
       <c r="C478" s="25" t="s">
-        <v>1006</v>
-      </c>
-      <c r="D478" s="25"/>
+        <v>1005</v>
+      </c>
+      <c r="D478" s="25" t="s">
+        <v>638</v>
+      </c>
       <c r="E478" s="25"/>
       <c r="F478" s="25" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="479" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A479" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B479" s="66" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C479" s="25" t="s">
-        <v>679</v>
-      </c>
-      <c r="D479" s="25" t="s">
-        <v>510</v>
-      </c>
-      <c r="E479" s="25"/>
-      <c r="F479" s="25" t="s">
-        <v>1020</v>
-      </c>
+        <v>680</v>
+      </c>
+      <c r="C479" s="51" t="s">
+        <v>541</v>
+      </c>
+      <c r="D479" s="51"/>
+      <c r="E479" s="51"/>
+      <c r="F479" s="51"/>
     </row>
     <row r="480" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A480" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B480" s="66" t="s">
-        <v>1008</v>
-      </c>
-      <c r="C480" s="25" t="s">
-        <v>1005</v>
+        <v>681</v>
+      </c>
+      <c r="C480" s="32" t="s">
+        <v>543</v>
       </c>
       <c r="D480" s="25" t="s">
-        <v>638</v>
-      </c>
-      <c r="E480" s="25"/>
+        <v>520</v>
+      </c>
+      <c r="E480" s="32"/>
       <c r="F480" s="25" t="s">
         <v>1020</v>
       </c>
@@ -12976,47 +12982,47 @@
         <v>55</v>
       </c>
       <c r="B481" s="66" t="s">
-        <v>680</v>
-      </c>
-      <c r="C481" s="51" t="s">
-        <v>541</v>
-      </c>
-      <c r="D481" s="51"/>
-      <c r="E481" s="51"/>
-      <c r="F481" s="51"/>
+        <v>682</v>
+      </c>
+      <c r="C481" s="25" t="s">
+        <v>545</v>
+      </c>
+      <c r="D481" s="25" t="s">
+        <v>988</v>
+      </c>
+      <c r="E481" s="25"/>
+      <c r="F481" s="25" t="s">
+        <v>1020</v>
+      </c>
     </row>
     <row r="482" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A482" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B482" s="66" t="s">
-        <v>681</v>
-      </c>
-      <c r="C482" s="32" t="s">
-        <v>543</v>
-      </c>
-      <c r="D482" s="25" t="s">
-        <v>520</v>
-      </c>
-      <c r="E482" s="32"/>
-      <c r="F482" s="25" t="s">
-        <v>1020</v>
-      </c>
+        <v>683</v>
+      </c>
+      <c r="C482" s="51" t="s">
+        <v>547</v>
+      </c>
+      <c r="D482" s="51"/>
+      <c r="E482" s="51"/>
+      <c r="F482" s="51"/>
     </row>
     <row r="483" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A483" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B483" s="66" t="s">
-        <v>682</v>
-      </c>
-      <c r="C483" s="25" t="s">
-        <v>545</v>
+        <v>684</v>
+      </c>
+      <c r="C483" s="32" t="s">
+        <v>514</v>
       </c>
       <c r="D483" s="25" t="s">
-        <v>988</v>
-      </c>
-      <c r="E483" s="25"/>
+        <v>515</v>
+      </c>
+      <c r="E483" s="32"/>
       <c r="F483" s="25" t="s">
         <v>1020</v>
       </c>
@@ -13026,27 +13032,31 @@
         <v>55</v>
       </c>
       <c r="B484" s="66" t="s">
-        <v>683</v>
-      </c>
-      <c r="C484" s="51" t="s">
-        <v>547</v>
-      </c>
-      <c r="D484" s="51"/>
-      <c r="E484" s="51"/>
-      <c r="F484" s="51"/>
+        <v>685</v>
+      </c>
+      <c r="C484" s="32" t="s">
+        <v>585</v>
+      </c>
+      <c r="D484" s="25" t="s">
+        <v>518</v>
+      </c>
+      <c r="E484" s="32"/>
+      <c r="F484" s="25" t="s">
+        <v>1020</v>
+      </c>
     </row>
     <row r="485" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A485" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B485" s="66" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="C485" s="32" t="s">
-        <v>514</v>
+        <v>552</v>
       </c>
       <c r="D485" s="25" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="E485" s="32"/>
       <c r="F485" s="25" t="s">
@@ -13058,15 +13068,15 @@
         <v>55</v>
       </c>
       <c r="B486" s="66" t="s">
-        <v>685</v>
-      </c>
-      <c r="C486" s="32" t="s">
-        <v>585</v>
+        <v>687</v>
+      </c>
+      <c r="C486" s="25" t="s">
+        <v>554</v>
       </c>
       <c r="D486" s="25" t="s">
-        <v>518</v>
-      </c>
-      <c r="E486" s="32"/>
+        <v>991</v>
+      </c>
+      <c r="E486" s="25"/>
       <c r="F486" s="25" t="s">
         <v>1020</v>
       </c>
@@ -13076,52 +13086,16 @@
         <v>55</v>
       </c>
       <c r="B487" s="66" t="s">
-        <v>686</v>
-      </c>
-      <c r="C487" s="32" t="s">
-        <v>552</v>
+        <v>1161</v>
+      </c>
+      <c r="C487" s="25" t="s">
+        <v>556</v>
       </c>
       <c r="D487" s="25" t="s">
-        <v>520</v>
-      </c>
-      <c r="E487" s="32"/>
+        <v>989</v>
+      </c>
+      <c r="E487" s="25"/>
       <c r="F487" s="25" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="488" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A488" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B488" s="66" t="s">
-        <v>687</v>
-      </c>
-      <c r="C488" s="25" t="s">
-        <v>554</v>
-      </c>
-      <c r="D488" s="25" t="s">
-        <v>991</v>
-      </c>
-      <c r="E488" s="25"/>
-      <c r="F488" s="25" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="489" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A489" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B489" s="66" t="s">
-        <v>1161</v>
-      </c>
-      <c r="C489" s="25" t="s">
-        <v>556</v>
-      </c>
-      <c r="D489" s="25" t="s">
-        <v>989</v>
-      </c>
-      <c r="E489" s="25"/>
-      <c r="F489" s="25" t="s">
         <v>1020</v>
       </c>
     </row>
@@ -14426,7 +14400,7 @@
         <v>711</v>
       </c>
       <c r="D6" s="63" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18" t="s">
@@ -14638,13 +14612,13 @@
         <v>1219</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>696</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -15133,7 +15107,7 @@
         <v>1051</v>
       </c>
       <c r="D43" s="62" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="E43" s="31"/>
       <c r="F43" s="18" t="s">
@@ -15152,7 +15126,7 @@
         <v>1052</v>
       </c>
       <c r="D44" s="62" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E44" s="31"/>
       <c r="F44" s="18" t="s">
@@ -15171,7 +15145,7 @@
         <v>1053</v>
       </c>
       <c r="D45" s="62" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="E45" s="31"/>
       <c r="F45" s="18" t="s">
@@ -15190,7 +15164,7 @@
         <v>1054</v>
       </c>
       <c r="D46" s="62" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="E46" s="31"/>
       <c r="F46" s="18" t="s">
@@ -15209,7 +15183,7 @@
         <v>1055</v>
       </c>
       <c r="D47" s="62" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="E47" s="31"/>
       <c r="F47" s="18" t="s">
@@ -15228,7 +15202,7 @@
         <v>1056</v>
       </c>
       <c r="D48" s="62" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="E48" s="31"/>
       <c r="F48" s="18" t="s">
@@ -15247,7 +15221,7 @@
         <v>1057</v>
       </c>
       <c r="D49" s="62" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="E49" s="31"/>
       <c r="F49" s="18" t="s">
@@ -15266,7 +15240,7 @@
         <v>1058</v>
       </c>
       <c r="D50" s="62" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="E50" s="31"/>
       <c r="F50" s="18" t="s">
@@ -15285,7 +15259,7 @@
         <v>1059</v>
       </c>
       <c r="D51" s="62" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="E51" s="31"/>
       <c r="F51" s="18" t="s">
@@ -15304,7 +15278,7 @@
         <v>1060</v>
       </c>
       <c r="D52" s="62" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="E52" s="31"/>
       <c r="F52" s="18" t="s">
@@ -15323,7 +15297,7 @@
         <v>1061</v>
       </c>
       <c r="D53" s="62" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="E53" s="31"/>
       <c r="F53" s="18" t="s">
@@ -15342,7 +15316,7 @@
         <v>1078</v>
       </c>
       <c r="D54" s="62" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="E54" s="31"/>
       <c r="F54" s="18" t="s">
@@ -18355,7 +18329,7 @@
         <v>1031</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>884</v>
@@ -18377,7 +18351,7 @@
         <v>902</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18" t="s">
@@ -18456,7 +18430,7 @@
         <v>909</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>910</v>
@@ -19492,10 +19466,10 @@
         <v>944</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>696</v>
@@ -19617,7 +19591,7 @@
         <v>696</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="14" spans="1:256" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -19728,7 +19702,7 @@
         <v>969</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="E19" s="24" t="s">
         <v>1141</v>
@@ -19751,7 +19725,7 @@
         <v>970</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="E20"/>
       <c r="F20" s="18" t="s">
@@ -19773,7 +19747,7 @@
         <v>972</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>696</v>

</xml_diff>